<commit_message>
results are currently outdated, requires new push
</commit_message>
<xml_diff>
--- a/Experiment Results.xlsx
+++ b/Experiment Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Paper Experiments" sheetId="1" state="visible" r:id="rId2"/>
@@ -443,9 +443,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>507240</xdr:colOff>
+      <xdr:colOff>506880</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>93240</xdr:rowOff>
+      <xdr:rowOff>92880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -459,7 +459,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11626560" y="606600"/>
-          <a:ext cx="4177800" cy="3713040"/>
+          <a:ext cx="4177440" cy="3712680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -485,9 +485,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>968760</xdr:colOff>
+      <xdr:colOff>968400</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>6480</xdr:rowOff>
+      <xdr:rowOff>6120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -501,7 +501,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="858240" y="4096080"/>
-          <a:ext cx="4177440" cy="3713040"/>
+          <a:ext cx="4177080" cy="3712680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -521,19 +521,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:66"/>
+  <dimension ref="A1:AMJ66"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F74" activeCellId="0" sqref="F74"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K33" activeCellId="0" sqref="K33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="32.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1216,15 +1216,6 @@
       <c r="H33" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="K33" s="0" t="n">
-        <v>4.962</v>
-      </c>
-      <c r="L33" s="0" t="n">
-        <v>0.119</v>
-      </c>
-      <c r="M33" s="0" t="n">
-        <v>0.842</v>
-      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="n">
@@ -1241,15 +1232,6 @@
       </c>
       <c r="H34" s="0" t="s">
         <v>30</v>
-      </c>
-      <c r="K34" s="0" t="n">
-        <v>4.713</v>
-      </c>
-      <c r="L34" s="0" t="n">
-        <v>0.117</v>
-      </c>
-      <c r="M34" s="0" t="n">
-        <v>85.2</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1974,7 +1956,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1990,15 +1972,15 @@
   </sheetPr>
   <dimension ref="A1:S17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="32.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2510,7 +2492,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>